<commit_message>
changed reading styling to be buttons
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1C9BBE-4C12-2445-A969-809DE5774F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874C2BE-635D-314E-BF65-67EE0AB2FFD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6940" yWindow="4200" windowWidth="25560" windowHeight="22980" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>assignments/#labs</t>
   </si>
   <si>
-    <t>Final Project</t>
-  </si>
-  <si>
     <t>Lab 1</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>lab-1</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -715,9 +715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F7" sqref="F7"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -758,22 +758,22 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -796,19 +796,19 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
@@ -826,10 +826,10 @@
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1">
         <v>22</v>
@@ -843,20 +843,20 @@
         <v>44207</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -867,26 +867,26 @@
         <v>44209</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -897,17 +897,17 @@
         <v>44214</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L6" s="1">
         <v>13</v>
@@ -921,23 +921,23 @@
         <v>44216</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -948,17 +948,17 @@
         <v>44221</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
@@ -972,29 +972,29 @@
         <v>44223</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="L9" s="1">
         <v>2</v>
@@ -1008,20 +1008,20 @@
         <v>44228</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1032,28 +1032,28 @@
         <v>44230</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="1">
         <v>6</v>
@@ -1067,20 +1067,20 @@
         <v>44235</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -1091,31 +1091,31 @@
         <v>44237</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="L13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1126,17 +1126,17 @@
         <v>44242</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="L14" s="1">
         <v>5</v>
@@ -1150,20 +1150,20 @@
         <v>44244</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="L15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1174,11 +1174,11 @@
         <v>44249</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -1189,25 +1189,25 @@
         <v>44251</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="J17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1218,21 +1218,21 @@
         <v>44256</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4"/>
       <c r="J18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1243,17 +1243,17 @@
         <v>44258</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1264,11 +1264,11 @@
         <v>44263</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="4"/>
     </row>
@@ -1280,11 +1280,11 @@
         <v>44265</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1295,16 +1295,16 @@
         <v>44272</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated reading for Week 1
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6DE586-A647-424F-A091-2AA0343F748B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E78057-2822-FE40-9184-5AF4FD01A2C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="1300" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="12300" yWindow="6120" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
   <si>
     <t>week</t>
   </si>
@@ -90,12 +90,6 @@
     <t>book_chapters</t>
   </si>
   <si>
-    <t>install-intro.html</t>
-  </si>
-  <si>
-    <t>4-8</t>
-  </si>
-  <si>
     <t>git-branches.html</t>
   </si>
   <si>
@@ -352,6 +346,9 @@
   </si>
   <si>
     <t>w1p2</t>
+  </si>
+  <si>
+    <t>https://www.sds.pub/collaborating-with-git-and-github.html</t>
   </si>
 </sst>
 </file>
@@ -395,11 +392,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -719,8 +716,8 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -776,7 +773,7 @@
         <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
@@ -790,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -799,19 +796,19 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
+      <c r="L2" s="5">
+        <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
@@ -824,8 +821,8 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>108</v>
+      <c r="D3" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -834,7 +831,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L3" s="1">
         <v>22</v>
@@ -848,20 +845,20 @@
         <v>44207</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -874,24 +871,24 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -902,17 +899,17 @@
         <v>44214</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L6" s="1">
         <v>13</v>
@@ -926,20 +923,20 @@
         <v>44216</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>13</v>
@@ -953,17 +950,17 @@
         <v>44221</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
@@ -979,9 +976,9 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
@@ -990,16 +987,16 @@
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L9" s="1">
         <v>2</v>
@@ -1013,20 +1010,20 @@
         <v>44228</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1037,28 +1034,28 @@
         <v>44230</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L11" s="1">
         <v>6</v>
@@ -1072,20 +1069,20 @@
         <v>44235</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="D12" s="4"/>
       <c r="E12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -1096,31 +1093,31 @@
         <v>44237</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -1131,17 +1128,17 @@
         <v>44242</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L14" s="1">
         <v>5</v>
@@ -1155,20 +1152,20 @@
         <v>44244</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1179,11 +1176,11 @@
         <v>44249</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -1194,25 +1191,25 @@
         <v>44251</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1223,21 +1220,21 @@
         <v>44256</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="F18" s="3"/>
       <c r="J18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1248,17 +1245,17 @@
         <v>44258</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1269,13 +1266,13 @@
         <v>44263</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1285,11 +1282,11 @@
         <v>44265</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1300,16 +1297,16 @@
         <v>44272</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
w3p2 video lecture link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F492AA-FF72-E444-AD5D-F5807468C184}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1268DFF5-A68C-864E-A4C5-2EAD08ECBD2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39360" yWindow="4920" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="26060" yWindow="4660" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
   <si>
     <t>week</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>https://youtu.be/qjpG75BByh4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/W2mCywkvGp4</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,6 +990,9 @@
       <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
minor edits to w4p1 and w4p2 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1268DFF5-A68C-864E-A4C5-2EAD08ECBD2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01494642-C3BC-AC44-8A5C-C6E1FB6A9F9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26060" yWindow="4660" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
   <si>
     <t>week</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>https://youtu.be/W2mCywkvGp4</t>
+  </si>
+  <si>
+    <t>w4p2</t>
   </si>
 </sst>
 </file>
@@ -754,9 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,7 +1033,9 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
fix error in rendering description of week 9b
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80334D8-96FF-4B4A-BAEC-5E9AF85411FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C34291-F4A1-F441-859A-D0630DC8B7C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26060" yWindow="4660" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>Loose ends and review</t>
   </si>
   <si>
-    <t>This course moves very fast. This is a designated "fudge" day to catch up on topics we either did not get to or covered too quickly the first time around. Assuming we have time, we will also review many of the core concepts of the course.</t>
-  </si>
-  <si>
     <t>assignments/#labs; assignments/#homework</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>https://youtu.be/UUxCl50aunk</t>
+  </si>
+  <si>
+    <t>This course moves very fast. This is a designated *fudge* day to catch up on topics we either did not get to or covered too quickly the first time around. Assuming we have time, we will also review many of the core concepts of the course.</t>
   </si>
 </sst>
 </file>
@@ -780,9 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,19 +861,19 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L2" s="5">
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -902,7 +902,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -916,7 +916,7 @@
         <v>58</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>59</v>
@@ -931,7 +931,7 @@
         <v>24</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -949,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
@@ -979,10 +979,10 @@
         <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="L6" s="1">
         <v>13</v>
@@ -999,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>34</v>
@@ -1011,13 +1011,13 @@
         <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1031,7 +1031,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>38</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -1060,10 +1060,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
@@ -1072,10 +1072,10 @@
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>41</v>
@@ -1087,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
@@ -1116,7 +1116,7 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>48</v>
@@ -1142,10 +1142,10 @@
         <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>41</v>
@@ -1168,19 +1168,19 @@
         <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -1194,10 +1194,10 @@
         <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>35</v>
@@ -1212,13 +1212,13 @@
         <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="L13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1232,16 +1232,16 @@
         <v>53</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="L14" s="1">
         <v>5</v>
@@ -1258,19 +1258,19 @@
         <v>52</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="L15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1299,10 +1299,10 @@
         <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>64</v>
@@ -1311,13 +1311,13 @@
         <v>65</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1331,20 +1331,20 @@
         <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="3"/>
       <c r="J18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -1359,13 +1359,13 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1410,13 +1410,13 @@
         <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
link to w6p1 lecture video
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C34291-F4A1-F441-859A-D0630DC8B7C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83518D1-F82A-2847-98FC-A1CC30529BFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26060" yWindow="4660" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="8400" yWindow="1840" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="127">
   <si>
     <t>week</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>This course moves very fast. This is a designated *fudge* day to catch up on topics we either did not get to or covered too quickly the first time around. Assuming we have time, we will also review many of the core concepts of the course.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/CaURv7EZVDk</t>
   </si>
 </sst>
 </file>
@@ -780,9 +783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,6 +1185,9 @@
       <c r="L12" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="M12" s="6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1422,6 +1428,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M8" r:id="rId1" xr:uid="{6D0F7BE9-D738-F14D-821A-7D1E4D6F8524}"/>
+    <hyperlink ref="M12" r:id="rId2" xr:uid="{E3FA1D02-A7B1-1C4D-A295-4303B8C8197E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
w6p2 lecture recording link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0EA08E-DA0B-174A-BB6F-CE75644CDFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C962D15F-20C0-B64B-8211-AA34865110CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8400" yWindow="1840" windowWidth="29440" windowHeight="19180" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="132">
   <si>
     <t>week</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>assignments/#draft; homework-2</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QdC033Ulu0s</t>
   </si>
 </sst>
 </file>
@@ -795,9 +798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,6 +1241,9 @@
       <c r="L13" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="M13" s="6" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1458,6 +1464,7 @@
   <hyperlinks>
     <hyperlink ref="M8" r:id="rId1" xr:uid="{6D0F7BE9-D738-F14D-821A-7D1E4D6F8524}"/>
     <hyperlink ref="M12" r:id="rId2" xr:uid="{E3FA1D02-A7B1-1C4D-A295-4303B8C8197E}"/>
+    <hyperlink ref="M13" r:id="rId3" xr:uid="{5F612834-1808-4248-9308-416FF4160206}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add link to Akhila's lecture
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D77B7-6D11-8D4C-971C-716EE7F62C30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA44FC96-3B44-B946-B89C-A1C90A158278}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="35820" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="133">
   <si>
     <t>week</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Building (static) data dashboards with the [{flexdashboard}](https://rmarkdown.rstudio.com/flexdashboard/) package. We'll discuss layouts, including multi-page layouts, storyboards, icons, and publishing through GitHub.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/dqRd0HPGtFA</t>
   </si>
 </sst>
 </file>
@@ -798,9 +801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,6 +1273,9 @@
       <c r="L14" s="1">
         <v>5</v>
       </c>
+      <c r="M14" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1465,6 +1471,7 @@
     <hyperlink ref="M8" r:id="rId1" xr:uid="{6D0F7BE9-D738-F14D-821A-7D1E4D6F8524}"/>
     <hyperlink ref="M12" r:id="rId2" xr:uid="{E3FA1D02-A7B1-1C4D-A295-4303B8C8197E}"/>
     <hyperlink ref="M13" r:id="rId3" xr:uid="{5F612834-1808-4248-9308-416FF4160206}"/>
+    <hyperlink ref="M14" r:id="rId4" xr:uid="{70665105-1881-1343-9BE8-49D9F24996DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
post w8p1 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E15C05-947C-844D-A7DC-148058D5526E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C80B83-948C-444D-A38D-B801AAA26ED1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="2080" windowWidth="33600" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="136">
   <si>
     <t>week</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>https://youtu.be/N01vfzx2abo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/z4xisZX5j3U</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M15" sqref="M15"/>
+      <selection pane="topRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,6 +1340,9 @@
       <c r="L16" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="M16" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="1">

</xml_diff>

<commit_message>
W9 slides and re-render PDFs for some reason
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c2-dataviz-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913C1FA-A7E2-1F41-B633-D2C0AB6D8579}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389D0109-F9A9-8544-A3AD-65DEB4BD2887}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="2080" windowWidth="33600" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="138">
   <si>
     <t>week</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>https://youtu.be/06qd_mUlvL4</t>
+  </si>
+  <si>
+    <t>w9p2</t>
   </si>
 </sst>
 </file>
@@ -813,9 +816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1428,9 @@
       <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>60</v>
       </c>

</xml_diff>